<commit_message>
last commit before ASC deprecation
</commit_message>
<xml_diff>
--- a/otros/Base de Datos ICI Thru.xlsx
+++ b/otros/Base de Datos ICI Thru.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gicsa\Desktop\Fichas GICSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arcad\Documents\Aztecatrol\CentralSoftware\otros\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5C0A7D-17BC-4CE4-B0EC-82A84FB63508}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB - ICI Thru" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -305,10 +314,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="170" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -407,13 +416,13 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -432,7 +441,7 @@
     <xf numFmtId="12" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -717,30 +726,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" style="18"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" customWidth="1"/>
+    <col min="9" max="9" width="19.77734375" customWidth="1"/>
+    <col min="10" max="10" width="18.21875" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" customWidth="1"/>
+    <col min="14" max="14" width="25.44140625" customWidth="1"/>
+    <col min="15" max="15" width="26" customWidth="1"/>
+    <col min="16" max="16" width="11.44140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -762,7 +775,7 @@
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
     </row>
-    <row r="2" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -814,7 +827,7 @@
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="3" t="s">
         <v>65</v>
@@ -871,7 +884,7 @@
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
         <v>66</v>
@@ -928,7 +941,7 @@
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="3" t="s">
         <v>67</v>
@@ -985,7 +998,7 @@
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="3" t="s">
         <v>68</v>
@@ -1042,7 +1055,7 @@
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="3" t="s">
         <v>69</v>
@@ -1099,7 +1112,7 @@
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="3" t="s">
         <v>70</v>
@@ -1156,7 +1169,7 @@
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="3" t="s">
         <v>71</v>
@@ -1213,7 +1226,7 @@
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="3" t="s">
         <v>72</v>
@@ -1270,7 +1283,7 @@
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="3" t="s">
         <v>73</v>
@@ -1327,7 +1340,7 @@
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="3" t="s">
         <v>74</v>
@@ -1384,7 +1397,7 @@
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
         <v>75</v>
@@ -1441,7 +1454,7 @@
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="3" t="s">
         <v>76</v>
@@ -1498,7 +1511,7 @@
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="3" t="s">
         <v>77</v>
@@ -1555,7 +1568,7 @@
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="3" t="s">
         <v>78</v>
@@ -1612,7 +1625,7 @@
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="3" t="s">
         <v>77</v>
@@ -1669,7 +1682,7 @@
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="3" t="s">
         <v>79</v>
@@ -1726,7 +1739,7 @@
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="3" t="s">
         <v>80</v>
@@ -1783,7 +1796,7 @@
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="3" t="s">
         <v>81</v>
@@ -1840,7 +1853,7 @@
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="3" t="s">
         <v>82</v>
@@ -1897,7 +1910,7 @@
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
         <v>83</v>
@@ -1953,7 +1966,7 @@
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="3" t="s">
         <v>84</v>
@@ -2010,7 +2023,7 @@
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="3" t="s">
         <v>85</v>
@@ -2066,7 +2079,7 @@
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="3" t="s">
         <v>86</v>
@@ -2123,7 +2136,7 @@
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="3" t="s">
         <v>87</v>
@@ -2180,7 +2193,7 @@
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="3" t="s">
         <v>88</v>
@@ -2236,7 +2249,7 @@
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="3" t="s">
         <v>89</v>
@@ -2292,7 +2305,7 @@
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="3" t="s">
         <v>90</v>
@@ -2348,7 +2361,7 @@
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="13" t="s">
         <v>39</v>
@@ -2405,7 +2418,7 @@
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="13" t="s">
         <v>40</v>
@@ -2462,7 +2475,7 @@
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="13" t="s">
         <v>41</v>
@@ -2519,7 +2532,7 @@
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="13" t="s">
         <v>42</v>
@@ -2576,7 +2589,7 @@
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="13" t="s">
         <v>43</v>
@@ -2633,7 +2646,7 @@
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="13" t="s">
         <v>44</v>
@@ -2690,7 +2703,7 @@
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="13" t="s">
         <v>45</v>
@@ -2747,7 +2760,7 @@
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="13" t="s">
         <v>46</v>
@@ -2804,7 +2817,7 @@
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="13" t="s">
         <v>47</v>
@@ -2861,7 +2874,7 @@
       <c r="S38" s="5"/>
       <c r="T38" s="5"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="13" t="s">
         <v>48</v>
@@ -2918,7 +2931,7 @@
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="13" t="s">
         <v>49</v>
@@ -2975,7 +2988,7 @@
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="13" t="s">
         <v>50</v>
@@ -3032,7 +3045,7 @@
       <c r="S41" s="5"/>
       <c r="T41" s="5"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="13" t="s">
         <v>51</v>
@@ -3089,7 +3102,7 @@
       <c r="S42" s="5"/>
       <c r="T42" s="5"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="13" t="s">
         <v>52</v>
@@ -3146,7 +3159,7 @@
       <c r="S43" s="5"/>
       <c r="T43" s="5"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="13" t="s">
         <v>51</v>
@@ -3203,7 +3216,7 @@
       <c r="S44" s="5"/>
       <c r="T44" s="5"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="13" t="s">
         <v>53</v>
@@ -3260,7 +3273,7 @@
       <c r="S45" s="5"/>
       <c r="T45" s="5"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="13" t="s">
         <v>54</v>
@@ -3317,7 +3330,7 @@
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="13" t="s">
         <v>55</v>
@@ -3374,7 +3387,7 @@
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="13" t="s">
         <v>56</v>
@@ -3431,7 +3444,7 @@
       <c r="S48" s="5"/>
       <c r="T48" s="5"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="13" t="s">
         <v>57</v>
@@ -3487,7 +3500,7 @@
       <c r="S49" s="5"/>
       <c r="T49" s="5"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="13" t="s">
         <v>58</v>
@@ -3544,7 +3557,7 @@
       <c r="S50" s="5"/>
       <c r="T50" s="5"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="13" t="s">
         <v>59</v>
@@ -3600,7 +3613,7 @@
       <c r="S51" s="5"/>
       <c r="T51" s="5"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="13" t="s">
         <v>60</v>
@@ -3657,7 +3670,7 @@
       <c r="S52" s="5"/>
       <c r="T52" s="5"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="13" t="s">
         <v>61</v>
@@ -3714,7 +3727,7 @@
       <c r="S53" s="5"/>
       <c r="T53" s="5"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="13" t="s">
         <v>62</v>
@@ -3770,7 +3783,7 @@
       <c r="S54" s="5"/>
       <c r="T54" s="5"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="13" t="s">
         <v>63</v>
@@ -3826,7 +3839,7 @@
       <c r="S55" s="5"/>
       <c r="T55" s="5"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="13" t="s">
         <v>64</v>
@@ -3882,7 +3895,7 @@
       <c r="S56" s="5"/>
       <c r="T56" s="5"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -3904,7 +3917,7 @@
       <c r="S57" s="5"/>
       <c r="T57" s="5"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -3926,7 +3939,7 @@
       <c r="S58" s="5"/>
       <c r="T58" s="5"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -3948,7 +3961,7 @@
       <c r="S59" s="5"/>
       <c r="T59" s="5"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>

</xml_diff>